<commit_message>
Output better, test crashing.
</commit_message>
<xml_diff>
--- a/tests/Unit/Roster/data/small.xlsx
+++ b/tests/Unit/Roster/data/small.xlsx
@@ -2965,7 +2965,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3067,10 +3067,10 @@
   <dimension ref="A2:AS603"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.66"/>
@@ -3389,7 +3389,9 @@
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
+      <c r="H10" s="36" t="n">
+        <v>0.333333333333333</v>
+      </c>
       <c r="I10" s="36"/>
       <c r="J10" s="37"/>
       <c r="K10" s="36"/>
@@ -3421,11 +3423,11 @@
       <c r="AK10" s="41"/>
       <c r="AL10" s="42" t="n">
         <f aca="false">COUNTIF(F100:AK101, "&gt;1")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM10" s="43" t="n">
         <f aca="false">SUM(F100:AK101)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AN10" s="44" t="n">
         <f aca="false">AO10*3.7</f>
@@ -3446,7 +3448,9 @@
       <c r="E11" s="33"/>
       <c r="F11" s="48"/>
       <c r="G11" s="49"/>
-      <c r="H11" s="50"/>
+      <c r="H11" s="50" t="n">
+        <v>0.833333333333333</v>
+      </c>
       <c r="I11" s="50"/>
       <c r="J11" s="51"/>
       <c r="K11" s="50"/>
@@ -7211,7 +7215,7 @@
       </c>
       <c r="H100" s="151" t="n">
         <f aca="false">MOD(H11-H10, 1)*24</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I100" s="151" t="n">
         <f aca="false">MOD(I11-I10, 1)*24</f>
@@ -30042,7 +30046,7 @@
       <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -30065,7 +30069,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -30088,7 +30092,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -30111,7 +30115,7 @@
       <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="160" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="161" width="8"/>
@@ -40812,7 +40816,7 @@
       <c r="B123" s="355"/>
       <c r="C123" s="371" t="n">
         <f aca="true">NOW()</f>
-        <v>45445.0515770499</v>
+        <v>45469.4106469046</v>
       </c>
       <c r="D123" s="371"/>
       <c r="E123" s="355"/>
@@ -41427,7 +41431,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="2" style="0" width="5.01"/>
@@ -41537,9 +41541,9 @@
         <f aca="false">IF('Darbo grafikas'!G9&lt;&gt;"",IF('Darbo grafikas'!G10&lt;&gt;"",IF('Darbo grafikas'!G9='Darbo grafikas'!G10,"",IF('Darbo grafikas'!G9&lt;'Darbo grafikas'!G10,('Darbo grafikas'!G10-'Darbo grafikas'!G9)*24,('Darbo grafikas'!G10-'Darbo grafikas'!G9+1)*24)),""),"")</f>
         <v/>
       </c>
-      <c r="C2" s="373" t="str">
+      <c r="C2" s="373" t="n">
         <f aca="false">IF('Darbo grafikas'!H9&lt;&gt;"",IF('Darbo grafikas'!H10&lt;&gt;"",IF('Darbo grafikas'!H9='Darbo grafikas'!H10,"",IF('Darbo grafikas'!H9&lt;'Darbo grafikas'!H10,('Darbo grafikas'!H10-'Darbo grafikas'!H9)*24,('Darbo grafikas'!H10-'Darbo grafikas'!H9+1)*24)),""),"")</f>
-        <v/>
+        <v>-40</v>
       </c>
       <c r="D2" s="373" t="str">
         <f aca="false">IF('Darbo grafikas'!I9&lt;&gt;"",IF('Darbo grafikas'!I10&lt;&gt;"",IF('Darbo grafikas'!I9='Darbo grafikas'!I10,"",IF('Darbo grafikas'!I9&lt;'Darbo grafikas'!I10,('Darbo grafikas'!I10-'Darbo grafikas'!I9)*24,('Darbo grafikas'!I10-'Darbo grafikas'!I9+1)*24)),""),"")</f>
@@ -41663,9 +41667,9 @@
         <f aca="false">IF('Darbo grafikas'!G10&lt;&gt;"",IF('Darbo grafikas'!G11&lt;&gt;"",IF('Darbo grafikas'!G10='Darbo grafikas'!G11,"",IF('Darbo grafikas'!G10&lt;'Darbo grafikas'!G11,('Darbo grafikas'!G11-'Darbo grafikas'!G10)*24,('Darbo grafikas'!G11-'Darbo grafikas'!G10+1)*24)),""),"")</f>
         <v/>
       </c>
-      <c r="C3" s="373" t="str">
+      <c r="C3" s="373" t="n">
         <f aca="false">IF('Darbo grafikas'!H10&lt;&gt;"",IF('Darbo grafikas'!H11&lt;&gt;"",IF('Darbo grafikas'!H10='Darbo grafikas'!H11,"",IF('Darbo grafikas'!H10&lt;'Darbo grafikas'!H11,('Darbo grafikas'!H11-'Darbo grafikas'!H10)*24,('Darbo grafikas'!H11-'Darbo grafikas'!H10+1)*24)),""),"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="D3" s="373" t="str">
         <f aca="false">IF('Darbo grafikas'!I10&lt;&gt;"",IF('Darbo grafikas'!I11&lt;&gt;"",IF('Darbo grafikas'!I10='Darbo grafikas'!I11,"",IF('Darbo grafikas'!I10&lt;'Darbo grafikas'!I11,('Darbo grafikas'!I11-'Darbo grafikas'!I10)*24,('Darbo grafikas'!I11-'Darbo grafikas'!I10+1)*24)),""),"")</f>
@@ -45456,7 +45460,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="149"/>

</xml_diff>